<commit_message>
checking all the formulas
</commit_message>
<xml_diff>
--- a/misc/app/Lipids_SLD_calculator.xlsx
+++ b/misc/app/Lipids_SLD_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anz/Documents/Andy/programming/refnx/misc/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/Andy/programming/refnx/misc/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F75676EC-4A9F-C242-87CE-74703E1065E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9DBC49-87B5-1A45-8B73-385BA07B2B07}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12680" yWindow="460" windowWidth="35620" windowHeight="11300" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14700" yWindow="1840" windowWidth="35620" windowHeight="11300" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="h-DMPC" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,14 @@
     <sheet name="HAPAK61GN1P" sheetId="36" r:id="rId37"/>
     <sheet name="d37OTS" sheetId="39" r:id="rId38"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3385,13 +3392,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3421,8 +3428,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1724025" y="1457325"/>
-          <a:ext cx="4267200" cy="1619250"/>
+          <a:off x="1905000" y="1444625"/>
+          <a:ext cx="4803775" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5236,7 +5243,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5317,30 +5324,30 @@
       </c>
       <c r="C2">
         <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
-        <v>255.16</v>
+        <v>269.16999999999996</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <f>((Q2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="F2">
         <f>((R2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="G2">
         <f>((S2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539683E-6</v>
       </c>
       <c r="H2">
         <f>((T2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="I2">
         <f>((U2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="J2">
         <v>7</v>
@@ -5355,7 +5362,7 @@
         <v>8</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -5365,23 +5372,23 @@
       </c>
       <c r="Q2">
         <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="R2">
         <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="S2">
         <f>((Q2*0.92)+(R2*0.08))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2578000000000005</v>
       </c>
       <c r="T2">
         <f>((Q2*0.62)+(R2*0.38))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="U2">
         <f>((Q2*0.34)+(R2*0.66))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -5470,7 +5477,7 @@
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
-        <v>704.12</v>
+        <v>718.12999999999988</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
@@ -5478,23 +5485,23 @@
       </c>
       <c r="E4">
         <f>((Q4/10000)/B4)</f>
-        <v>2.2198327759197318E-7</v>
+        <v>3.0024414715719058E-7</v>
       </c>
       <c r="F4">
         <f>((R4/10000)/B4)</f>
-        <v>2.2198327759197318E-7</v>
+        <v>3.0024414715719058E-7</v>
       </c>
       <c r="G4">
         <f>((S4/10000)/B4)</f>
-        <v>2.2198327759197318E-7</v>
+        <v>3.0024414715719068E-7</v>
       </c>
       <c r="H4">
         <f>((T4/10000)/B4)</f>
-        <v>2.2198327759197318E-7</v>
+        <v>3.0024414715719058E-7</v>
       </c>
       <c r="I4">
         <f>((U4/10000)/B4)</f>
-        <v>2.2198327759197318E-7</v>
+        <v>3.0024414715719058E-7</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -5514,7 +5521,7 @@
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
@@ -5526,23 +5533,23 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>2.6549199999999993</v>
+        <v>3.5909199999999992</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>2.6549199999999993</v>
+        <v>3.5909199999999992</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>2.6549199999999993</v>
+        <v>3.5909200000000001</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>2.6549199999999993</v>
+        <v>3.5909199999999992</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>2.6549199999999993</v>
+        <v>3.5909199999999992</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -5571,7 +5578,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5652,30 +5659,30 @@
       </c>
       <c r="C2">
         <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
-        <v>255.16</v>
+        <v>269.16999999999996</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <f>((Q2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="F2">
         <f>((R2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="G2">
         <f>((S2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539683E-6</v>
       </c>
       <c r="H2">
         <f>((T2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="I2">
         <f>((U2/10000)/B2)</f>
-        <v>2.1118253968253964E-6</v>
+        <v>2.4832539682539679E-6</v>
       </c>
       <c r="J2">
         <v>7</v>
@@ -5690,7 +5697,7 @@
         <v>8</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -5700,23 +5707,23 @@
       </c>
       <c r="Q2">
         <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="R2">
         <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="S2">
         <f>((Q2*0.92)+(R2*0.08))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2578000000000005</v>
       </c>
       <c r="T2">
         <f>((Q2*0.62)+(R2*0.38))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
       <c r="U2">
         <f>((Q2*0.34)+(R2*0.66))</f>
-        <v>5.3217999999999996</v>
+        <v>6.2577999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -5805,7 +5812,7 @@
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
-        <v>735.43</v>
+        <v>749.43999999999994</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
@@ -5813,23 +5820,23 @@
       </c>
       <c r="E4">
         <f>((Q4/10000)/B4)</f>
-        <v>2.921497491638796E-6</v>
+        <v>2.9997583612040135E-6</v>
       </c>
       <c r="F4">
         <f>((R4/10000)/B4)</f>
-        <v>2.921497491638796E-6</v>
+        <v>2.9997583612040135E-6</v>
       </c>
       <c r="G4">
         <f>((S4/10000)/B4)</f>
-        <v>2.921497491638796E-6</v>
+        <v>2.9997583612040135E-6</v>
       </c>
       <c r="H4">
         <f>((T4/10000)/B4)</f>
-        <v>2.9214974916387965E-6</v>
+        <v>2.9997583612040135E-6</v>
       </c>
       <c r="I4">
         <f>((U4/10000)/B4)</f>
-        <v>2.9214974916387965E-6</v>
+        <v>2.9997583612040135E-6</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -5849,7 +5856,7 @@
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
@@ -5861,23 +5868,23 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>34.941110000000002</v>
+        <v>35.877110000000002</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>34.941110000000002</v>
+        <v>35.877110000000002</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>34.941110000000002</v>
+        <v>35.877110000000002</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>34.941110000000009</v>
+        <v>35.877110000000002</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>34.941110000000009</v>
+        <v>35.877110000000002</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -5906,7 +5913,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5987,30 +5994,30 @@
       </c>
       <c r="C2">
         <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
-        <v>259.2</v>
+        <v>273.20999999999998</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2">
         <f>((Q2/10000)/B2)</f>
-        <v>3.7649841269841263E-6</v>
+        <v>4.1364126984126973E-6</v>
       </c>
       <c r="F2" s="2">
         <f>((R2/10000)/B2)</f>
-        <v>5.0048531746031754E-6</v>
+        <v>5.3762817460317461E-6</v>
       </c>
       <c r="G2">
         <f>((S2/10000)/B2)</f>
-        <v>3.8641736507936497E-6</v>
+        <v>4.235602222222222E-6</v>
       </c>
       <c r="H2">
         <f>((T2/10000)/B2)</f>
-        <v>4.2361343650793645E-6</v>
+        <v>4.6075629365079368E-6</v>
       </c>
       <c r="I2">
         <f>((U2/10000)/B2)</f>
-        <v>4.5832976984126979E-6</v>
+        <v>4.9547262698412702E-6</v>
       </c>
       <c r="J2">
         <v>7</v>
@@ -6025,7 +6032,7 @@
         <v>8</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -6035,23 +6042,23 @@
       </c>
       <c r="Q2">
         <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>9.487759999999998</v>
+        <v>10.423759999999998</v>
       </c>
       <c r="R2">
         <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>12.61223</v>
+        <v>13.54823</v>
       </c>
       <c r="S2">
         <f>((Q2*0.92)+(R2*0.08))</f>
-        <v>9.7377175999999981</v>
+        <v>10.6737176</v>
       </c>
       <c r="T2">
         <f>((Q2*0.62)+(R2*0.38))</f>
-        <v>10.6750586</v>
+        <v>11.6110586</v>
       </c>
       <c r="U2">
         <f>((Q2*0.34)+(R2*0.66))</f>
-        <v>11.549910199999999</v>
+        <v>12.485910200000001</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -6140,7 +6147,7 @@
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
-        <v>708.16</v>
+        <v>722.17</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
@@ -6148,23 +6155,23 @@
       </c>
       <c r="E4">
         <f>((Q4/10000)/B4)</f>
-        <v>5.7030769230769205E-7</v>
+        <v>6.485685618729095E-7</v>
       </c>
       <c r="F4">
         <f>((R4/10000)/B4)</f>
-        <v>8.3155100334448157E-7</v>
+        <v>9.0981187290969891E-7</v>
       </c>
       <c r="G4">
         <f>((S4/10000)/B4)</f>
-        <v>5.9120715719063522E-7</v>
+        <v>6.6946802675585277E-7</v>
       </c>
       <c r="H4">
         <f>((T4/10000)/B4)</f>
-        <v>6.6958015050167221E-7</v>
+        <v>7.4784102006688956E-7</v>
       </c>
       <c r="I4">
         <f>((U4/10000)/B4)</f>
-        <v>7.4272827759197309E-7</v>
+        <v>8.2098914715719065E-7</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -6184,7 +6191,7 @@
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
@@ -6196,23 +6203,23 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>6.8208799999999972</v>
+        <v>7.7568799999999971</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>9.9453499999999995</v>
+        <v>10.881349999999999</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>7.0708375999999973</v>
+        <v>8.006837599999999</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>8.008178599999999</v>
+        <v>8.944178599999999</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>8.8830301999999985</v>
+        <v>9.8190302000000003</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -6911,7 +6918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
@@ -10174,7 +10181,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10250,36 +10257,36 @@
       </c>
       <c r="C2">
         <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
-        <v>558.30999999999995</v>
+        <v>554.27</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>((Q2/10000)/B2)</f>
-        <v>2.9080988142292485E-6</v>
+        <v>3.2038221343873517E-6</v>
       </c>
       <c r="F2">
         <f>((R2/10000)/B2)</f>
-        <v>3.1139268774703556E-6</v>
+        <v>3.4096501976284576E-6</v>
       </c>
       <c r="G2">
         <f>((S2/10000)/B2)</f>
-        <v>2.924565059288537E-6</v>
+        <v>3.2202883794466402E-6</v>
       </c>
       <c r="H2">
         <f>((T2/10000)/B2)</f>
-        <v>2.9863134782608689E-6</v>
+        <v>3.2820367984189717E-6</v>
       </c>
       <c r="I2">
         <f>((U2/10000)/B2)</f>
-        <v>3.0439453359683793E-6</v>
+        <v>3.3396686561264817E-6</v>
       </c>
       <c r="J2">
         <v>17</v>
       </c>
       <c r="K2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -10298,23 +10305,23 @@
       </c>
       <c r="Q2">
         <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>14.714979999999997</v>
+        <v>16.21134</v>
       </c>
       <c r="R2">
         <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>15.756469999999998</v>
+        <v>17.252829999999996</v>
       </c>
       <c r="S2">
         <f>((Q2*0.92)+(R2*0.08))</f>
-        <v>14.798299199999997</v>
+        <v>16.294659199999998</v>
       </c>
       <c r="T2">
         <f>((Q2*0.62)+(R2*0.38))</f>
-        <v>15.110746199999998</v>
+        <v>16.607106199999997</v>
       </c>
       <c r="U2">
         <f>((Q2*0.34)+(R2*0.66))</f>
-        <v>15.402363399999999</v>
+        <v>16.898723399999998</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -10326,36 +10333,36 @@
       </c>
       <c r="C3">
         <f>((J3*12.01)+(K3*1.01)+(L3*2.02)+(M3*16)+(N3*14.01)+(O3*30.97)+(P3*32.06))</f>
-        <v>689.6</v>
+        <v>685.56000000000006</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <f>((Q3/10000)/B3)</f>
-        <v>-6.3441931385006351E-7</v>
+        <v>-5.3935196950444721E-7</v>
       </c>
       <c r="F3">
         <f>((R3/10000)/B3)</f>
-        <v>-6.3441931385006351E-7</v>
+        <v>-5.3935196950444721E-7</v>
       </c>
       <c r="G3">
         <f>((S3/10000)/B3)</f>
-        <v>-6.3441931385006351E-7</v>
+        <v>-5.3935196950444721E-7</v>
       </c>
       <c r="H3">
         <f>((T3/10000)/B3)</f>
-        <v>-6.3441931385006351E-7</v>
+        <v>-5.3935196950444721E-7</v>
       </c>
       <c r="I3">
         <f>((U3/10000)/B3)</f>
-        <v>-6.3441931385006351E-7</v>
+        <v>-5.3935196950444721E-7</v>
       </c>
       <c r="J3">
         <v>48</v>
       </c>
       <c r="K3">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -10374,23 +10381,23 @@
       </c>
       <c r="Q3">
         <f>(((J3*6.6484)+(K3*-3.7409)+(L3*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
-        <v>-9.9857599999999991</v>
+        <v>-8.4893999999999998</v>
       </c>
       <c r="R3">
         <f>(((J3*6.6484)+((K3-D3)*-3.7409)+((L3+D3)*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
-        <v>-9.9857599999999991</v>
+        <v>-8.4893999999999998</v>
       </c>
       <c r="S3">
         <f>((Q3*0.92)+(R3*0.08))</f>
-        <v>-9.9857599999999991</v>
+        <v>-8.4893999999999998</v>
       </c>
       <c r="T3">
         <f>((Q3*0.62)+(R3*0.38))</f>
-        <v>-9.9857599999999991</v>
+        <v>-8.4893999999999998</v>
       </c>
       <c r="U3">
         <f>((Q3*0.34)+(R3*0.66))</f>
-        <v>-9.9857599999999991</v>
+        <v>-8.4893999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -10403,7 +10410,7 @@
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
-        <v>1247.9099999999999</v>
+        <v>1239.83</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
@@ -10411,23 +10418,23 @@
       </c>
       <c r="E4">
         <f>((Q4/10000)/B4)</f>
-        <v>2.2736634615384605E-7</v>
+        <v>3.7124711538461538E-7</v>
       </c>
       <c r="F4">
         <f>((R4/10000)/B4)</f>
-        <v>2.7743798076923075E-7</v>
+        <v>4.2131874999999982E-7</v>
       </c>
       <c r="G4">
         <f>((S4/10000)/B4)</f>
-        <v>2.3137207692307684E-7</v>
+        <v>3.7525284615384604E-7</v>
       </c>
       <c r="H4">
         <f>((T4/10000)/B4)</f>
-        <v>2.4639356730769223E-7</v>
+        <v>3.902743365384614E-7</v>
       </c>
       <c r="I4">
         <f>((U4/10000)/B4)</f>
-        <v>2.6041362499999995E-7</v>
+        <v>4.0429439423076913E-7</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -10435,7 +10442,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -10459,23 +10466,23 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>4.729219999999998</v>
+        <v>7.72194</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>5.7707099999999993</v>
+        <v>8.7634299999999961</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>4.812539199999998</v>
+        <v>7.8052591999999983</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>5.1249861999999986</v>
+        <v>8.1177061999999971</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>5.4166033999999996</v>
+        <v>8.4093233999999981</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
@@ -10498,8 +10505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10575,36 +10582,36 @@
       </c>
       <c r="C2">
         <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
-        <v>558.30999999999995</v>
+        <v>506.22999999999996</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>((Q2/10000)/B2)</f>
-        <v>2.9080988142292485E-6</v>
+        <v>2.6782569169960475E-6</v>
       </c>
       <c r="F2">
         <f>((R2/10000)/B2)</f>
-        <v>3.1139268774703556E-6</v>
+        <v>2.8840849802371542E-6</v>
       </c>
       <c r="G2">
         <f>((S2/10000)/B2)</f>
-        <v>2.924565059288537E-6</v>
+        <v>2.694723162055336E-6</v>
       </c>
       <c r="H2">
         <f>((T2/10000)/B2)</f>
-        <v>2.9863134782608689E-6</v>
+        <v>2.7564715810276678E-6</v>
       </c>
       <c r="I2">
         <f>((U2/10000)/B2)</f>
-        <v>3.0439453359683793E-6</v>
+        <v>2.8141034387351779E-6</v>
       </c>
       <c r="J2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -10623,23 +10630,23 @@
       </c>
       <c r="Q2">
         <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>14.714979999999997</v>
+        <v>13.55198</v>
       </c>
       <c r="R2">
         <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
-        <v>15.756469999999998</v>
+        <v>14.59347</v>
       </c>
       <c r="S2">
         <f>((Q2*0.92)+(R2*0.08))</f>
-        <v>14.798299199999997</v>
+        <v>13.6352992</v>
       </c>
       <c r="T2">
         <f>((Q2*0.62)+(R2*0.38))</f>
-        <v>15.110746199999998</v>
+        <v>13.947746200000001</v>
       </c>
       <c r="U2">
         <f>((Q2*0.34)+(R2*0.66))</f>
-        <v>15.402363399999999</v>
+        <v>14.2393634</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -10728,7 +10735,7 @@
       </c>
       <c r="C4">
         <f>SUM(C2:C3)</f>
-        <v>1508.31</v>
+        <v>1456.23</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
@@ -10736,31 +10743,31 @@
       </c>
       <c r="E4">
         <f>((Q4/10000)/B4)</f>
-        <v>4.2620129345189957E-7</v>
+        <v>3.7919240097008886E-7</v>
       </c>
       <c r="F4">
         <f>((R4/10000)/B4)</f>
-        <v>4.6829870654810014E-7</v>
+        <v>4.2128981406628932E-7</v>
       </c>
       <c r="G4">
         <f>((S4/10000)/B4)</f>
-        <v>4.2956908649959567E-7</v>
+        <v>3.8256019401778491E-7</v>
       </c>
       <c r="H4">
         <f>((T4/10000)/B4)</f>
-        <v>4.4219831042845577E-7</v>
+        <v>3.9518941794664512E-7</v>
       </c>
       <c r="I4">
         <f>((U4/10000)/B4)</f>
-        <v>4.5398558609539198E-7</v>
+        <v>4.0697669361358122E-7</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -10784,23 +10791,23 @@
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>10.544219999999996</v>
+        <v>9.381219999999999</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>11.585709999999997</v>
+        <v>10.422709999999999</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>10.627539199999996</v>
+        <v>9.464539199999999</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>10.939986199999996</v>
+        <v>9.7769861999999996</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>11.231603399999997</v>
+        <v>10.068603399999999</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -12883,7 +12890,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17185,7 +17192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ENH: add more lipids to database
</commit_message>
<xml_diff>
--- a/misc/app/Lipids_SLD_calculator.xlsx
+++ b/misc/app/Lipids_SLD_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/Andy/programming/refnx/misc/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anz/Documents/Andy/programming/refnx/misc/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100348A4-058F-DF45-865E-D3FAFC430B1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED63D409-0180-C24C-B5CD-C0991803F7F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25360" yWindow="680" windowWidth="35620" windowHeight="11300" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="680" windowWidth="35620" windowHeight="11300" firstSheet="24" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="h-DMPC" sheetId="1" r:id="rId1"/>
@@ -51,20 +51,16 @@
     <sheet name="PAPAKB61GN1P" sheetId="35" r:id="rId36"/>
     <sheet name="HAPAK61GN1P" sheetId="36" r:id="rId37"/>
     <sheet name="d37OTS" sheetId="39" r:id="rId38"/>
+    <sheet name="h-DOPC" sheetId="41" r:id="rId39"/>
+    <sheet name="DOTAP" sheetId="43" r:id="rId40"/>
+    <sheet name="18_1 Diether PC" sheetId="42" r:id="rId41"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="80">
   <si>
     <t>Heads</t>
   </si>
@@ -989,6 +985,30 @@
   <si>
     <t>O=COCC(COP(=O)([O-])OC1C(O)C(O)C(OP(=O)(O)[O-])C(OP(=O)(O)[O-])C1O)OC=O,-5.73,311.07,33,547.17,19,5,2,14,386.02</t>
   </si>
+  <si>
+    <t>Greenwood et al. Chem Phys Lipids. 2006 September ; 143(1-2): 1–10. doi:10.1016/j.chemphyslip.2006.04.002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kucerka et al.  J. Membrane Biol. 208, 193 - 202 (2005)</t>
+  </si>
+  <si>
+    <t>Tristram-Nagle et al, Biophysical Journal Volume 75 August 1998 917–925</t>
+  </si>
+  <si>
+    <t>Also subtract C=O from HG.</t>
+  </si>
+  <si>
+    <t>No Carbonyl in headgroup.  Therefore add 2 x CH2 to tails.</t>
+  </si>
+  <si>
+    <t>Armen et al.  Biophysical Journal Volume 75 August 1998 734–744</t>
+  </si>
+  <si>
+    <t>Calculations based on DOPC.  Adjustments made to headgroup regions on the basis of MD calculations.</t>
+  </si>
+  <si>
+    <t>Based on DOPC as for DiEther DOPC</t>
+  </si>
 </sst>
 </file>
 
@@ -1045,11 +1065,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3187,6 +3208,138 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing38.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="18:1 (Δ9-Cis) PC (DOPC)">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C069A2B2-E787-1A46-A088-DD7E887065A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="977900" y="1346200"/>
+          <a:ext cx="7620000" cy="1346200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>11642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="18:1 TAP (DOTAP)">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{759EE432-536C-7447-914B-C85F5C26B2A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="774700" y="1308100"/>
+          <a:ext cx="6578600" cy="1370542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3250,6 +3403,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7620000" cy="927100"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="18:1 Diether PC">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D67DCAD-A523-A744-895C-151BDE97153D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1651000" y="1574800"/>
+          <a:ext cx="7620000" cy="927100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8537,7 +8751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -16197,6 +16411,347 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDBA569-51E6-A34D-95BA-1EA0E3C84202}">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>319</v>
+      </c>
+      <c r="C2">
+        <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
+        <v>311.26</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>((Q2/10000)/B2)</f>
+        <v>1.8833166144200629E-6</v>
+      </c>
+      <c r="F2">
+        <f>((R2/10000)/B2)</f>
+        <v>1.8833166144200629E-6</v>
+      </c>
+      <c r="G2">
+        <f>((S2/10000)/B2)</f>
+        <v>1.8833166144200629E-6</v>
+      </c>
+      <c r="H2">
+        <f>((T2/10000)/B2)</f>
+        <v>1.8833166144200629E-6</v>
+      </c>
+      <c r="I2">
+        <f>((U2/10000)/B2)</f>
+        <v>1.8833166144200629E-6</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>6.0077800000000003</v>
+      </c>
+      <c r="R2">
+        <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>6.0077800000000003</v>
+      </c>
+      <c r="S2">
+        <f>((Q2*0.92)+(R2*0.08))</f>
+        <v>6.0077800000000003</v>
+      </c>
+      <c r="T2">
+        <f>((Q2*0.62)+(R2*0.38))</f>
+        <v>6.0077800000000003</v>
+      </c>
+      <c r="U2">
+        <f>((Q2*0.34)+(R2*0.66))</f>
+        <v>6.0077800000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>1294-B2</f>
+        <v>975</v>
+      </c>
+      <c r="C3">
+        <f>((J3*12.01)+(K3*1.01)+(L3*2.02)+(M3*16)+(N3*14.01)+(O3*30.97)+(P3*32.06))</f>
+        <v>475</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>((Q3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="F3">
+        <f>((R3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="G3">
+        <f>((S3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="H3">
+        <f>((T3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="I3">
+        <f>((U3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="J3">
+        <v>34</v>
+      </c>
+      <c r="K3">
+        <v>66</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>(((J3*6.6484)+(K3*-3.7409)+(L3*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="R3">
+        <f>(((J3*6.6484)+((K3-D3)*-3.7409)+((L3+D3)*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="S3">
+        <f>((Q3*0.92)+(R3*0.08))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="T3">
+        <f>((Q3*0.62)+(R3*0.38))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="U3">
+        <f>((Q3*0.34)+(R3*0.66))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2:B3)</f>
+        <v>1294</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>786.26</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>((Q4/10000)/B4)</f>
+        <v>3.0312210200927356E-7</v>
+      </c>
+      <c r="F4">
+        <f>((R4/10000)/B4)</f>
+        <v>3.0312210200927356E-7</v>
+      </c>
+      <c r="G4">
+        <f>((S4/10000)/B4)</f>
+        <v>3.0312210200927356E-7</v>
+      </c>
+      <c r="H4">
+        <f>((T4/10000)/B4)</f>
+        <v>3.0312210200927356E-7</v>
+      </c>
+      <c r="I4">
+        <f>((U4/10000)/B4)</f>
+        <v>3.0312210200927356E-7</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>3.9223999999999997</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>3.9223999999999997</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>3.9223999999999997</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>3.9223999999999997</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>3.9223999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U22"/>
@@ -16524,6 +17079,679 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7179B6AA-516D-3649-AC08-549548CA6D29}">
+  <dimension ref="A1:U20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>319-53.7-56</f>
+        <v>209.3</v>
+      </c>
+      <c r="C2">
+        <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
+        <v>188.23</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>((Q2/10000)/B2)</f>
+        <v>1.5955375059722886E-6</v>
+      </c>
+      <c r="F2">
+        <f>((R2/10000)/B2)</f>
+        <v>1.5955375059722886E-6</v>
+      </c>
+      <c r="G2">
+        <f>((S2/10000)/B2)</f>
+        <v>1.5955375059722886E-6</v>
+      </c>
+      <c r="H2">
+        <f>((T2/10000)/B2)</f>
+        <v>1.5955375059722886E-6</v>
+      </c>
+      <c r="I2">
+        <f>((U2/10000)/B2)</f>
+        <v>1.5955375059722886E-6</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>3.3394599999999999</v>
+      </c>
+      <c r="R2">
+        <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>3.3394599999999999</v>
+      </c>
+      <c r="S2">
+        <f>((Q2*0.92)+(R2*0.08))</f>
+        <v>3.3394599999999999</v>
+      </c>
+      <c r="T2">
+        <f>((Q2*0.62)+(R2*0.38))</f>
+        <v>3.3394599999999999</v>
+      </c>
+      <c r="U2">
+        <f>((Q2*0.34)+(R2*0.66))</f>
+        <v>3.3394599999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>975</v>
+      </c>
+      <c r="C3">
+        <f>((J3*12.01)+(K3*1.01)+(L3*2.02)+(M3*16)+(N3*14.01)+(O3*30.97)+(P3*32.06))</f>
+        <v>475</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>((Q3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="F3">
+        <f>((R3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="G3">
+        <f>((S3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="H3">
+        <f>((T3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="I3">
+        <f>((U3/10000)/B3)</f>
+        <v>-2.1388512820512827E-7</v>
+      </c>
+      <c r="J3">
+        <v>34</v>
+      </c>
+      <c r="K3">
+        <v>66</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>(((J3*6.6484)+(K3*-3.7409)+(L3*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="R3">
+        <f>(((J3*6.6484)+((K3-D3)*-3.7409)+((L3+D3)*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="S3">
+        <f>((Q3*0.92)+(R3*0.08))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="T3">
+        <f>((Q3*0.62)+(R3*0.38))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+      <c r="U3">
+        <f>((Q3*0.34)+(R3*0.66))</f>
+        <v>-2.0853800000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2:B3)</f>
+        <v>1184.3</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>663.23</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:U4" si="0">SUM(D2:D3)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>((Q4/10000)/B4)</f>
+        <v>1.0589208815333947E-7</v>
+      </c>
+      <c r="F4">
+        <f>((R4/10000)/B4)</f>
+        <v>1.0589208815333947E-7</v>
+      </c>
+      <c r="G4">
+        <f>((S4/10000)/B4)</f>
+        <v>1.0589208815333947E-7</v>
+      </c>
+      <c r="H4">
+        <f>((T4/10000)/B4)</f>
+        <v>1.0589208815333947E-7</v>
+      </c>
+      <c r="I4">
+        <f>((U4/10000)/B4)</f>
+        <v>1.0589208815333947E-7</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:P4" si="1">SUM(J2:J3)</f>
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>1.2540799999999992</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>1.2540799999999992</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>1.2540799999999992</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>1.2540799999999992</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>1.2540799999999992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F173495-B41F-FD43-890A-067F54EEADA2}">
+  <dimension ref="A1:U22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>319-28</f>
+        <v>291</v>
+      </c>
+      <c r="C2">
+        <f>((J2*12.01)+(K2*1.01)+(L2*2.02)+(M2*16)+(N2*14.01)+(O2*30.97)+(P2*32.06))</f>
+        <v>255.23999999999998</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>((Q2/10000)/B2)</f>
+        <v>1.2086254295532647E-6</v>
+      </c>
+      <c r="F2">
+        <f>((R2/10000)/B2)</f>
+        <v>1.2086254295532647E-6</v>
+      </c>
+      <c r="G2">
+        <f>((S2/10000)/B2)</f>
+        <v>1.2086254295532647E-6</v>
+      </c>
+      <c r="H2">
+        <f>((T2/10000)/B2)</f>
+        <v>1.2086254295532647E-6</v>
+      </c>
+      <c r="I2">
+        <f>((U2/10000)/B2)</f>
+        <v>1.208625429553265E-6</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>(((J2*6.6484)+(K2*-3.7409)+(L2*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>3.5171000000000006</v>
+      </c>
+      <c r="R2">
+        <f>(((J2*6.6484)+((K2-D2)*-3.7409)+((L2+D2)*6.674)+(M2*5.805)+(N2*9.36)+(O2*5.13)+(P2*2.8471))/10)</f>
+        <v>3.5171000000000006</v>
+      </c>
+      <c r="S2">
+        <f>((Q2*0.92)+(R2*0.08))</f>
+        <v>3.5171000000000006</v>
+      </c>
+      <c r="T2">
+        <f>((Q2*0.62)+(R2*0.38))</f>
+        <v>3.5171000000000006</v>
+      </c>
+      <c r="U2">
+        <f>((Q2*0.34)+(R2*0.66))</f>
+        <v>3.517100000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>980 + 56 + 2*28.1</f>
+        <v>1092.2</v>
+      </c>
+      <c r="C3">
+        <f>((J3*12.01)+(K3*1.01)+(L3*2.02)+(M3*16)+(N3*14.01)+(O3*30.97)+(P3*32.06))</f>
+        <v>503.06</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>((Q3/10000)/B3)</f>
+        <v>-2.0619483611060245E-7</v>
+      </c>
+      <c r="F3">
+        <f>((R3/10000)/B3)</f>
+        <v>-2.0619483611060245E-7</v>
+      </c>
+      <c r="G3">
+        <f>((S3/10000)/B3)</f>
+        <v>-2.0619483611060245E-7</v>
+      </c>
+      <c r="H3">
+        <f>((T3/10000)/B3)</f>
+        <v>-2.0619483611060245E-7</v>
+      </c>
+      <c r="I3">
+        <f>((U3/10000)/B3)</f>
+        <v>-2.0619483611060245E-7</v>
+      </c>
+      <c r="J3">
+        <v>36</v>
+      </c>
+      <c r="K3">
+        <v>70</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>(((J3*6.6484)+(K3*-3.7409)+(L3*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.2520600000000002</v>
+      </c>
+      <c r="R3">
+        <f>(((J3*6.6484)+((K3-D3)*-3.7409)+((L3+D3)*6.674)+(M3*5.805)+(N3*9.36)+(O3*5.13)+(P3*2.8471))/10)</f>
+        <v>-2.2520600000000002</v>
+      </c>
+      <c r="S3">
+        <f>((Q3*0.92)+(R3*0.08))</f>
+        <v>-2.2520600000000002</v>
+      </c>
+      <c r="T3">
+        <f>((Q3*0.62)+(R3*0.38))</f>
+        <v>-2.2520600000000002</v>
+      </c>
+      <c r="U3">
+        <f>((Q3*0.34)+(R3*0.66))</f>
+        <v>-2.2520600000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2:B3)</f>
+        <v>1383.2</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>758.3</v>
+      </c>
+      <c r="D4">
+        <f>SUM(D2:D3)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>((Q4/10000)/B4)</f>
+        <v>9.1457489878542543E-8</v>
+      </c>
+      <c r="F4">
+        <f>((R4/10000)/B4)</f>
+        <v>9.1457489878542543E-8</v>
+      </c>
+      <c r="G4">
+        <f>((S4/10000)/B4)</f>
+        <v>9.1457489878542543E-8</v>
+      </c>
+      <c r="H4">
+        <f>((T4/10000)/B4)</f>
+        <v>9.1457489878542543E-8</v>
+      </c>
+      <c r="I4">
+        <f>((U4/10000)/B4)</f>
+        <v>9.1457489878542556E-8</v>
+      </c>
+      <c r="J4">
+        <f>SUM(J2:J3)</f>
+        <v>44</v>
+      </c>
+      <c r="K4">
+        <f>SUM(K2:K3)</f>
+        <v>88</v>
+      </c>
+      <c r="L4">
+        <f>SUM(L2:L3)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>SUM(M2:M3)</f>
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <f>SUM(N2:N3)</f>
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f>SUM(O2:O3)</f>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f>SUM(P2:P3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f>SUM(Q2:Q3)</f>
+        <v>1.2650400000000004</v>
+      </c>
+      <c r="R4">
+        <f>SUM(R2:R3)</f>
+        <v>1.2650400000000004</v>
+      </c>
+      <c r="S4">
+        <f>SUM(S2:S3)</f>
+        <v>1.2650400000000004</v>
+      </c>
+      <c r="T4">
+        <f>SUM(T2:T3)</f>
+        <v>1.2650400000000004</v>
+      </c>
+      <c r="U4">
+        <f>SUM(U2:U3)</f>
+        <v>1.2650400000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>